<commit_message>
Removed semicolon from initial .xlsx files
</commit_message>
<xml_diff>
--- a/data/initial/staff_list.xlsx
+++ b/data/initial/staff_list.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sengy\Desktop\Workspace\School\NTU\SC2002 (OOP)\sc2002-project\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sengy\Desktop\Workspace\School\NTU\SC2002 (OOP)\sc2002-project\data\initial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9450597D-285C-4255-A7D4-F4CD7189D49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{A1AB1725-9614-4760-9E35-FCE78E076BF2}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="11025"/>
   </bookViews>
   <sheets>
     <sheet name="staff" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">staff!$A$1:$B$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">staff!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -79,9 +78,6 @@
     <t>UPAM@NTU.EDU.SG</t>
   </si>
   <si>
-    <t>OURIN@ntu.edu.sg</t>
-  </si>
-  <si>
     <t>HUKUMAR@NTU.EDU.SG</t>
   </si>
   <si>
@@ -89,12 +85,15 @@
   </si>
   <si>
     <t>Arvind</t>
+  </si>
+  <si>
+    <t>OURIN@NTU.EDU.SG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -481,22 +480,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55DE67C8-F00F-4E71-A7B2-83068F640C77}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" style="4" customWidth="1"/>
-    <col min="2" max="2" width="25.54296875" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -507,29 +506,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -540,7 +539,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -551,9 +550,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>10</v>
@@ -564,11 +563,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{81D093B7-7D45-4C94-BB5C-7AACAE95581C}"/>
-    <hyperlink ref="B5" r:id="rId2" xr:uid="{9931FE22-2FDA-4031-AC32-E8C581BFEA0B}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{C6203F7B-B631-4F6A-ABDC-A4C27A0A1DAD}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{49DFE096-5F31-4004-8F65-766F1044AD00}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{0B389DC2-D438-4218-8936-76A694EA9F12}"/>
+    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B3" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>

</xml_diff>

<commit_message>
completed java doc for UI
</commit_message>
<xml_diff>
--- a/data/initial/staff_list.xlsx
+++ b/data/initial/staff_list.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sengy\Desktop\Workspace\School\NTU\SC2002 (OOP)\sc2002-project\data\initial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01282f950008d7ec/Documents/NTU/ObjectOrientedProgramming/sc2002-project/data/initial/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_861630E143EB5BDE157423E7D7397ACABA8EC8A8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DFB41DA-5B65-4D4F-9BE8-99321701D270}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="11025"/>
+    <workbookView xWindow="16455" yWindow="150" windowWidth="11820" windowHeight="12765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="staff" sheetId="1" r:id="rId1"/>
@@ -23,15 +24,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -93,7 +85,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -480,7 +472,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -563,11 +555,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-    <hyperlink ref="B5" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B3" r:id="rId4"/>
-    <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>

</xml_diff>